<commit_message>
Starting another hard level
</commit_message>
<xml_diff>
--- a/2025 Excel Esports Chille - OR(TRICK, TREAT) (Juan Jose Cifuentes) - Case and Answers.xlsx
+++ b/2025 Excel Esports Chille - OR(TRICK, TREAT) (Juan Jose Cifuentes) - Case and Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700AFD70-AA34-434E-BC5F-BCE17BFA2059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D26471B-0251-4230-B9E6-5192DBAB483F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D933904C-08DE-4507-8D89-8C098F48A748}"/>
   </bookViews>
@@ -3784,6 +3784,12 @@
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="64" fillId="11" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="65" fillId="12" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="66" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3803,24 +3809,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="63" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3862,10 +3850,22 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="64" fillId="11" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="65" fillId="12" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="66" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="63" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4809,8 +4809,8 @@
   <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:BJ327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P309" sqref="P309"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G246" sqref="B243:G246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -4835,39 +4835,39 @@
   <sheetData>
     <row r="1" spans="2:51" ht="15" customHeight="1"/>
     <row r="2" spans="2:51" ht="59.25" customHeight="1">
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="190" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193"/>
-      <c r="L2" s="193"/>
-      <c r="M2" s="194"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="192"/>
     </row>
     <row r="3" spans="2:51" ht="15" customHeight="1"/>
     <row r="4" spans="2:51" ht="33" customHeight="1">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="187" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="185"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="189"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="183" t="s">
+      <c r="L4" s="187" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="185"/>
+      <c r="M4" s="189"/>
     </row>
     <row r="5" spans="2:51" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -4915,10 +4915,10 @@
       <c r="AY5"/>
     </row>
     <row r="6" spans="2:51" ht="33" customHeight="1">
-      <c r="L6" s="183" t="s">
+      <c r="L6" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="185"/>
+      <c r="M6" s="189"/>
     </row>
     <row r="7" spans="2:51" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -4926,52 +4926,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:51" ht="21.75" customHeight="1">
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="196"/>
-      <c r="K8" s="196"/>
-      <c r="L8" s="196"/>
-      <c r="M8" s="196"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="194"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="194"/>
+      <c r="L8" s="194"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="2:51" ht="162" customHeight="1">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="195" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="197"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="197"/>
-      <c r="M9" s="197"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
+      <c r="I9" s="195"/>
+      <c r="J9" s="195"/>
+      <c r="K9" s="195"/>
+      <c r="L9" s="195"/>
+      <c r="M9" s="195"/>
     </row>
     <row r="10" spans="2:51" ht="245.4" customHeight="1">
-      <c r="B10" s="198" t="s">
+      <c r="B10" s="196" t="s">
         <v>727</v>
       </c>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="198"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="198"/>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
-      <c r="K10" s="198"/>
-      <c r="L10" s="198"/>
-      <c r="M10" s="198"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="196"/>
+      <c r="J10" s="196"/>
+      <c r="K10" s="196"/>
+      <c r="L10" s="196"/>
+      <c r="M10" s="196"/>
     </row>
     <row r="11" spans="2:51" ht="15" customHeight="1">
       <c r="B11" s="5"/>
@@ -4988,20 +4988,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:51" ht="21.75" customHeight="1">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="187" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="185"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="188"/>
+      <c r="I12" s="188"/>
+      <c r="J12" s="188"/>
+      <c r="K12" s="188"/>
+      <c r="L12" s="188"/>
+      <c r="M12" s="189"/>
     </row>
     <row r="13" spans="2:51" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -5051,15 +5051,15 @@
         <v>86</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="199" t="s">
+      <c r="G16" s="197" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="200"/>
-      <c r="I16" s="200"/>
-      <c r="J16" s="200"/>
-      <c r="K16" s="200"/>
-      <c r="L16" s="200"/>
-      <c r="M16" s="201"/>
+      <c r="H16" s="198"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="198"/>
+      <c r="K16" s="198"/>
+      <c r="L16" s="198"/>
+      <c r="M16" s="199"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="16" t="s">
@@ -5073,15 +5073,15 @@
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="202" t="s">
+      <c r="G17" s="200" t="s">
         <v>732</v>
       </c>
-      <c r="H17" s="202"/>
-      <c r="I17" s="202"/>
-      <c r="J17" s="202"/>
-      <c r="K17" s="202"/>
-      <c r="L17" s="202"/>
-      <c r="M17" s="202"/>
+      <c r="H17" s="200"/>
+      <c r="I17" s="200"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="200"/>
+      <c r="M17" s="200"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="16" t="s">
@@ -5095,15 +5095,15 @@
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="179"/>
-      <c r="J18" s="179"/>
-      <c r="K18" s="179"/>
-      <c r="L18" s="179"/>
-      <c r="M18" s="179"/>
+      <c r="H18" s="183"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="183"/>
+      <c r="K18" s="183"/>
+      <c r="L18" s="183"/>
+      <c r="M18" s="183"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="16" t="s">
@@ -5117,15 +5117,15 @@
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="179" t="s">
+      <c r="G19" s="183" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="179"/>
-      <c r="I19" s="179"/>
-      <c r="J19" s="179"/>
-      <c r="K19" s="179"/>
-      <c r="L19" s="179"/>
-      <c r="M19" s="179"/>
+      <c r="H19" s="183"/>
+      <c r="I19" s="183"/>
+      <c r="J19" s="183"/>
+      <c r="K19" s="183"/>
+      <c r="L19" s="183"/>
+      <c r="M19" s="183"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="16" t="s">
@@ -5139,15 +5139,15 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="179" t="s">
+      <c r="G20" s="183" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="179"/>
-      <c r="I20" s="179"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="179"/>
-      <c r="L20" s="179"/>
-      <c r="M20" s="179"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+      <c r="K20" s="183"/>
+      <c r="L20" s="183"/>
+      <c r="M20" s="183"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="16" t="s">
@@ -5161,34 +5161,34 @@
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="180" t="s">
+      <c r="G21" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="J21" s="181"/>
-      <c r="K21" s="181"/>
-      <c r="L21" s="181"/>
-      <c r="M21" s="182"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
+      <c r="M21" s="186"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="187" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="184"/>
-      <c r="D23" s="184"/>
-      <c r="E23" s="184"/>
-      <c r="F23" s="184"/>
-      <c r="G23" s="184"/>
-      <c r="H23" s="184"/>
-      <c r="I23" s="184"/>
-      <c r="J23" s="184"/>
-      <c r="K23" s="184"/>
-      <c r="L23" s="184"/>
-      <c r="M23" s="185"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
+      <c r="K23" s="188"/>
+      <c r="L23" s="188"/>
+      <c r="M23" s="189"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -9195,7 +9195,7 @@
       <c r="G122" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H122" s="205" t="s">
+      <c r="H122" s="179" t="s">
         <v>144</v>
       </c>
       <c r="I122" s="170">
@@ -9221,11 +9221,11 @@
         <v>132</v>
       </c>
       <c r="P122" s="170" t="str">
-        <f>ADDRESS(N122,3)</f>
+        <f t="shared" ref="P122:P141" si="0">ADDRESS(N122,3)</f>
         <v>$C$3</v>
       </c>
       <c r="Q122" s="170" t="str">
-        <f>ADDRESS(N122,39)</f>
+        <f t="shared" ref="Q122:Q141" si="1">ADDRESS(N122,39)</f>
         <v>$AM$3</v>
       </c>
       <c r="R122" s="170">
@@ -9278,22 +9278,22 @@
       <c r="E123" s="42"/>
       <c r="F123" s="20"/>
       <c r="G123" s="43"/>
-      <c r="H123" s="205" t="s">
+      <c r="H123" s="179" t="s">
         <v>750</v>
       </c>
       <c r="I123" s="170">
         <v>7</v>
       </c>
       <c r="J123" s="170" t="str">
-        <f t="shared" ref="J123:J141" si="0">ADDRESS(3,I123)</f>
+        <f t="shared" ref="J123:J141" si="2">ADDRESS(3,I123)</f>
         <v>$G$3</v>
       </c>
       <c r="K123" s="170" t="str">
-        <f t="shared" ref="K123:K141" si="1">ADDRESS(41,I123)</f>
+        <f t="shared" ref="K123:K141" si="3">ADDRESS(41,I123)</f>
         <v>$G$41</v>
       </c>
       <c r="L123" s="170">
-        <f t="shared" ref="L123:L141" ca="1" si="2">COUNTIFS(INDIRECT("CellVille!"&amp;J123&amp;":"&amp;K123),$I$121)</f>
+        <f t="shared" ref="L123:L141" ca="1" si="4">COUNTIFS(INDIRECT("CellVille!"&amp;J123&amp;":"&amp;K123),$I$121)</f>
         <v>0</v>
       </c>
       <c r="M123" s="45"/>
@@ -9304,15 +9304,15 @@
         <v>141</v>
       </c>
       <c r="P123" s="170" t="str">
-        <f>ADDRESS(N123,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$8</v>
       </c>
       <c r="Q123" s="170" t="str">
-        <f>ADDRESS(N123,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$8</v>
       </c>
       <c r="R123" s="170">
-        <f t="shared" ref="R123:R141" ca="1" si="3">COUNTIFS(INDIRECT("CellVille!"&amp;P123&amp;":"&amp;Q123),$I$121)</f>
+        <f t="shared" ref="R123:R141" ca="1" si="5">COUNTIFS(INDIRECT("CellVille!"&amp;P123&amp;":"&amp;Q123),$I$121)</f>
         <v>0</v>
       </c>
       <c r="S123" s="45"/>
@@ -9372,22 +9372,22 @@
       <c r="G124" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="H124" s="205" t="s">
+      <c r="H124" s="179" t="s">
         <v>147</v>
       </c>
       <c r="I124" s="170">
         <v>12</v>
       </c>
       <c r="J124" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$L$3</v>
       </c>
       <c r="K124" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$L$41</v>
       </c>
       <c r="L124" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M124" s="170"/>
@@ -9398,15 +9398,15 @@
         <v>140</v>
       </c>
       <c r="P124" s="170" t="str">
-        <f>ADDRESS(N124,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$12</v>
       </c>
       <c r="Q124" s="170" t="str">
-        <f>ADDRESS(N124,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$12</v>
       </c>
       <c r="R124" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S124" s="170"/>
@@ -9466,22 +9466,22 @@
       <c r="G125" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H125" s="205" t="s">
+      <c r="H125" s="179" t="s">
         <v>131</v>
       </c>
       <c r="I125" s="170">
         <v>16</v>
       </c>
       <c r="J125" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$P$3</v>
       </c>
       <c r="K125" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$P$41</v>
       </c>
       <c r="L125" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M125" s="170"/>
@@ -9492,15 +9492,15 @@
         <v>230</v>
       </c>
       <c r="P125" s="170" t="str">
-        <f>ADDRESS(N125,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$16</v>
       </c>
       <c r="Q125" s="170" t="str">
-        <f>ADDRESS(N125,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$16</v>
       </c>
       <c r="R125" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S125" s="170"/>
@@ -9560,22 +9560,22 @@
       <c r="G126" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H126" s="205" t="s">
+      <c r="H126" s="179" t="s">
         <v>751</v>
       </c>
       <c r="I126" s="170">
         <v>19</v>
       </c>
       <c r="J126" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$S$3</v>
       </c>
       <c r="K126" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$S$41</v>
       </c>
       <c r="L126" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M126" s="170"/>
@@ -9586,15 +9586,15 @@
         <v>775</v>
       </c>
       <c r="P126" s="170" t="str">
-        <f>ADDRESS(N126,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$19</v>
       </c>
       <c r="Q126" s="170" t="str">
-        <f>ADDRESS(N126,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$19</v>
       </c>
       <c r="R126" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="S126" s="170"/>
@@ -9654,22 +9654,22 @@
       <c r="G127" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H127" s="205" t="s">
+      <c r="H127" s="179" t="s">
         <v>752</v>
       </c>
       <c r="I127" s="170">
         <v>22</v>
       </c>
       <c r="J127" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$V$3</v>
       </c>
       <c r="K127" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$V$41</v>
       </c>
       <c r="L127" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M127" s="170"/>
@@ -9680,15 +9680,15 @@
         <v>133</v>
       </c>
       <c r="P127" s="170" t="str">
-        <f>ADDRESS(N127,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$24</v>
       </c>
       <c r="Q127" s="170" t="str">
-        <f>ADDRESS(N127,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$24</v>
       </c>
       <c r="R127" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="S127" s="170"/>
@@ -9748,22 +9748,22 @@
       <c r="G128" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="H128" s="205" t="s">
+      <c r="H128" s="179" t="s">
         <v>136</v>
       </c>
       <c r="I128" s="170">
         <v>27</v>
       </c>
       <c r="J128" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AA$3</v>
       </c>
       <c r="K128" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AA$41</v>
       </c>
       <c r="L128" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M128" s="170"/>
@@ -9774,15 +9774,15 @@
         <v>776</v>
       </c>
       <c r="P128" s="170" t="str">
-        <f>ADDRESS(N128,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$27</v>
       </c>
       <c r="Q128" s="170" t="str">
-        <f>ADDRESS(N128,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$27</v>
       </c>
       <c r="R128" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S128" s="170"/>
@@ -9842,22 +9842,22 @@
       <c r="G129" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="H129" s="205" t="s">
+      <c r="H129" s="179" t="s">
         <v>228</v>
       </c>
       <c r="I129" s="170">
         <v>30</v>
       </c>
       <c r="J129" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AD$3</v>
       </c>
       <c r="K129" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AD$41</v>
       </c>
       <c r="L129" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M129" s="170"/>
@@ -9868,15 +9868,15 @@
         <v>146</v>
       </c>
       <c r="P129" s="170" t="str">
-        <f>ADDRESS(N129,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$31</v>
       </c>
       <c r="Q129" s="170" t="str">
-        <f>ADDRESS(N129,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$31</v>
       </c>
       <c r="R129" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S129" s="170"/>
@@ -9936,22 +9936,22 @@
       <c r="G130" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="H130" s="205" t="s">
+      <c r="H130" s="179" t="s">
         <v>142</v>
       </c>
       <c r="I130" s="170">
         <v>33</v>
       </c>
       <c r="J130" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AG$3</v>
       </c>
       <c r="K130" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AG$41</v>
       </c>
       <c r="L130" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M130" s="170"/>
@@ -9962,15 +9962,15 @@
         <v>226</v>
       </c>
       <c r="P130" s="170" t="str">
-        <f>ADDRESS(N130,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$36</v>
       </c>
       <c r="Q130" s="170" t="str">
-        <f>ADDRESS(N130,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$36</v>
       </c>
       <c r="R130" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="S130" s="170"/>
@@ -10030,22 +10030,22 @@
       <c r="G131" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H131" s="205" t="s">
+      <c r="H131" s="179" t="s">
         <v>225</v>
       </c>
       <c r="I131" s="170">
         <v>37</v>
       </c>
       <c r="J131" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AK$3</v>
       </c>
       <c r="K131" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AK$41</v>
       </c>
       <c r="L131" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M131" s="170"/>
@@ -10056,15 +10056,15 @@
         <v>739</v>
       </c>
       <c r="P131" s="170" t="str">
-        <f>ADDRESS(N131,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$39</v>
       </c>
       <c r="Q131" s="170" t="str">
-        <f>ADDRESS(N131,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$39</v>
       </c>
       <c r="R131" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S131" s="170"/>
@@ -10131,15 +10131,15 @@
         <v>5</v>
       </c>
       <c r="J132" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$E$3</v>
       </c>
       <c r="K132" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$E$41</v>
       </c>
       <c r="L132" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M132" s="170"/>
@@ -10150,15 +10150,15 @@
         <v>138</v>
       </c>
       <c r="P132" s="170" t="str">
-        <f>ADDRESS(N132,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$5</v>
       </c>
       <c r="Q132" s="170" t="str">
-        <f>ADDRESS(N132,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$5</v>
       </c>
       <c r="R132" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S132" s="170"/>
@@ -10225,15 +10225,15 @@
         <v>9</v>
       </c>
       <c r="J133" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$I$3</v>
       </c>
       <c r="K133" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$I$41</v>
       </c>
       <c r="L133" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="M133" s="170"/>
@@ -10244,15 +10244,15 @@
         <v>145</v>
       </c>
       <c r="P133" s="170" t="str">
-        <f>ADDRESS(N133,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$10</v>
       </c>
       <c r="Q133" s="170" t="str">
-        <f>ADDRESS(N133,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$10</v>
       </c>
       <c r="R133" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S133" s="170"/>
@@ -10319,15 +10319,15 @@
         <v>14</v>
       </c>
       <c r="J134" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$N$3</v>
       </c>
       <c r="K134" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$N$41</v>
       </c>
       <c r="L134" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M134" s="170"/>
@@ -10338,15 +10338,15 @@
         <v>777</v>
       </c>
       <c r="P134" s="170" t="str">
-        <f>ADDRESS(N134,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$14</v>
       </c>
       <c r="Q134" s="170" t="str">
-        <f>ADDRESS(N134,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$14</v>
       </c>
       <c r="R134" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S134" s="170"/>
@@ -10413,15 +10413,15 @@
         <v>18</v>
       </c>
       <c r="J135" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$R$3</v>
       </c>
       <c r="K135" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$R$41</v>
       </c>
       <c r="L135" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M135" s="170"/>
@@ -10432,15 +10432,15 @@
         <v>738</v>
       </c>
       <c r="P135" s="170" t="str">
-        <f>ADDRESS(N135,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$18</v>
       </c>
       <c r="Q135" s="170" t="str">
-        <f>ADDRESS(N135,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$18</v>
       </c>
       <c r="R135" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S135" s="170"/>
@@ -10509,15 +10509,15 @@
         <v>21</v>
       </c>
       <c r="J136" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$U$3</v>
       </c>
       <c r="K136" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$U$41</v>
       </c>
       <c r="L136" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M136" s="170"/>
@@ -10528,15 +10528,15 @@
         <v>229</v>
       </c>
       <c r="P136" s="170" t="str">
-        <f>ADDRESS(N136,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$21</v>
       </c>
       <c r="Q136" s="170" t="str">
-        <f>ADDRESS(N136,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$21</v>
       </c>
       <c r="R136" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S136" s="170"/>
@@ -10605,15 +10605,15 @@
         <v>24</v>
       </c>
       <c r="J137" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$X$3</v>
       </c>
       <c r="K137" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$X$41</v>
       </c>
       <c r="L137" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M137" s="170"/>
@@ -10624,15 +10624,15 @@
         <v>148</v>
       </c>
       <c r="P137" s="170" t="str">
-        <f>ADDRESS(N137,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$26</v>
       </c>
       <c r="Q137" s="170" t="str">
-        <f>ADDRESS(N137,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$26</v>
       </c>
       <c r="R137" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="S137" s="170"/>
@@ -10701,15 +10701,15 @@
         <v>29</v>
       </c>
       <c r="J138" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AC$3</v>
       </c>
       <c r="K138" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AC$41</v>
       </c>
       <c r="L138" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M138" s="170"/>
@@ -10720,15 +10720,15 @@
         <v>227</v>
       </c>
       <c r="P138" s="170" t="str">
-        <f>ADDRESS(N138,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$29</v>
       </c>
       <c r="Q138" s="170" t="str">
-        <f>ADDRESS(N138,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$29</v>
       </c>
       <c r="R138" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="S138" s="170"/>
@@ -10797,15 +10797,15 @@
         <v>32</v>
       </c>
       <c r="J139" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AF$3</v>
       </c>
       <c r="K139" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AF$41</v>
       </c>
       <c r="L139" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="M139" s="170"/>
@@ -10816,15 +10816,15 @@
         <v>135</v>
       </c>
       <c r="P139" s="170" t="str">
-        <f>ADDRESS(N139,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$33</v>
       </c>
       <c r="Q139" s="170" t="str">
-        <f>ADDRESS(N139,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$33</v>
       </c>
       <c r="R139" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S139" s="170"/>
@@ -10893,15 +10893,15 @@
         <v>35</v>
       </c>
       <c r="J140" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AI$3</v>
       </c>
       <c r="K140" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AI$41</v>
       </c>
       <c r="L140" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M140" s="170"/>
@@ -10912,15 +10912,15 @@
         <v>740</v>
       </c>
       <c r="P140" s="170" t="str">
-        <f>ADDRESS(N140,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$38</v>
       </c>
       <c r="Q140" s="170" t="str">
-        <f>ADDRESS(N140,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$38</v>
       </c>
       <c r="R140" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S140" s="170"/>
@@ -10989,15 +10989,15 @@
         <v>39</v>
       </c>
       <c r="J141" s="170" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>$AM$3</v>
       </c>
       <c r="K141" s="170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>$AM$41</v>
       </c>
       <c r="L141" s="170">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M141" s="170"/>
@@ -11008,15 +11008,15 @@
         <v>778</v>
       </c>
       <c r="P141" s="170" t="str">
-        <f>ADDRESS(N141,3)</f>
+        <f t="shared" si="0"/>
         <v>$C$41</v>
       </c>
       <c r="Q141" s="170" t="str">
-        <f>ADDRESS(N141,39)</f>
+        <f t="shared" si="1"/>
         <v>$AM$41</v>
       </c>
       <c r="R141" s="170">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="S141" s="170"/>
@@ -11276,20 +11276,20 @@
       <c r="K147" s="67"/>
     </row>
     <row r="148" spans="1:62" ht="23.4">
-      <c r="B148" s="183" t="s">
+      <c r="B148" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="C148" s="184"/>
-      <c r="D148" s="184"/>
-      <c r="E148" s="184"/>
-      <c r="F148" s="184"/>
-      <c r="G148" s="184"/>
-      <c r="H148" s="184"/>
-      <c r="I148" s="184"/>
-      <c r="J148" s="184"/>
-      <c r="K148" s="184"/>
-      <c r="L148" s="184"/>
-      <c r="M148" s="185"/>
+      <c r="C148" s="188"/>
+      <c r="D148" s="188"/>
+      <c r="E148" s="188"/>
+      <c r="F148" s="188"/>
+      <c r="G148" s="188"/>
+      <c r="H148" s="188"/>
+      <c r="I148" s="188"/>
+      <c r="J148" s="188"/>
+      <c r="K148" s="188"/>
+      <c r="L148" s="188"/>
+      <c r="M148" s="189"/>
     </row>
     <row r="149" spans="1:62" ht="15" customHeight="1" thickBot="1">
       <c r="B149" s="24"/>
@@ -15094,20 +15094,20 @@
       <c r="K232" s="67"/>
     </row>
     <row r="233" spans="1:62" ht="23.4">
-      <c r="B233" s="183" t="s">
+      <c r="B233" s="187" t="s">
         <v>211</v>
       </c>
-      <c r="C233" s="184"/>
-      <c r="D233" s="184"/>
-      <c r="E233" s="184"/>
-      <c r="F233" s="184"/>
-      <c r="G233" s="184"/>
-      <c r="H233" s="184"/>
-      <c r="I233" s="184"/>
-      <c r="J233" s="184"/>
-      <c r="K233" s="184"/>
-      <c r="L233" s="184"/>
-      <c r="M233" s="185"/>
+      <c r="C233" s="188"/>
+      <c r="D233" s="188"/>
+      <c r="E233" s="188"/>
+      <c r="F233" s="188"/>
+      <c r="G233" s="188"/>
+      <c r="H233" s="188"/>
+      <c r="I233" s="188"/>
+      <c r="J233" s="188"/>
+      <c r="K233" s="188"/>
+      <c r="L233" s="188"/>
+      <c r="M233" s="189"/>
     </row>
     <row r="234" spans="1:62" ht="15" customHeight="1" thickBot="1">
       <c r="B234" s="24"/>
@@ -18689,11 +18689,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G20:M20"/>
-    <mergeCell ref="G21:M21"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B148:M148"/>
-    <mergeCell ref="B233:M233"/>
     <mergeCell ref="G19:M19"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B4:J4"/>
@@ -18706,6 +18701,11 @@
     <mergeCell ref="G16:M16"/>
     <mergeCell ref="G17:M17"/>
     <mergeCell ref="G18:M18"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B148:M148"/>
+    <mergeCell ref="B233:M233"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19071,401 +19071,401 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="16384" width="8.796875" style="205"/>
+    <col min="1" max="16384" width="8.796875" style="179"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="181" t="s">
         <v>749</v>
       </c>
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="180" t="s">
         <v>748</v>
       </c>
-      <c r="C1" s="206"/>
+      <c r="C1" s="180"/>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="181" t="s">
         <v>747</v>
       </c>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
     </row>
     <row r="3" spans="1:39">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="181" t="s">
         <v>746</v>
       </c>
-      <c r="B3" s="206" t="str" cm="1">
+      <c r="B3" s="180" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
         <v>28-Oct-2025</v>
       </c>
-      <c r="C3" s="206"/>
+      <c r="C3" s="180"/>
     </row>
     <row r="7" spans="1:39" ht="14.4" thickBot="1"/>
     <row r="8" spans="1:39">
-      <c r="E8" s="208" t="s">
+      <c r="E8" s="182" t="s">
         <v>318</v>
       </c>
-      <c r="F8" s="208"/>
-      <c r="G8" s="208"/>
-      <c r="H8" s="208"/>
-      <c r="I8" s="208" t="s">
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182" t="s">
         <v>319</v>
       </c>
-      <c r="J8" s="208"/>
-      <c r="K8" s="208"/>
-      <c r="L8" s="208"/>
-      <c r="M8" s="208"/>
-      <c r="N8" s="208" t="s">
+      <c r="J8" s="182"/>
+      <c r="K8" s="182"/>
+      <c r="L8" s="182"/>
+      <c r="M8" s="182"/>
+      <c r="N8" s="182" t="s">
         <v>320</v>
       </c>
-      <c r="O8" s="208"/>
-      <c r="P8" s="208"/>
-      <c r="Q8" s="208"/>
-      <c r="R8" s="208" t="s">
+      <c r="O8" s="182"/>
+      <c r="P8" s="182"/>
+      <c r="Q8" s="182"/>
+      <c r="R8" s="182" t="s">
         <v>321</v>
       </c>
-      <c r="S8" s="208"/>
-      <c r="T8" s="208"/>
-      <c r="U8" s="208" t="s">
+      <c r="S8" s="182"/>
+      <c r="T8" s="182"/>
+      <c r="U8" s="182" t="s">
         <v>322</v>
       </c>
-      <c r="V8" s="208"/>
-      <c r="W8" s="208"/>
-      <c r="X8" s="208" t="s">
+      <c r="V8" s="182"/>
+      <c r="W8" s="182"/>
+      <c r="X8" s="182" t="s">
         <v>323</v>
       </c>
-      <c r="Y8" s="208"/>
-      <c r="Z8" s="208"/>
-      <c r="AA8" s="208"/>
-      <c r="AB8" s="208"/>
-      <c r="AC8" s="208" t="s">
+      <c r="Y8" s="182"/>
+      <c r="Z8" s="182"/>
+      <c r="AA8" s="182"/>
+      <c r="AB8" s="182"/>
+      <c r="AC8" s="182" t="s">
         <v>324</v>
       </c>
-      <c r="AD8" s="208"/>
-      <c r="AE8" s="208"/>
-      <c r="AF8" s="208" t="s">
+      <c r="AD8" s="182"/>
+      <c r="AE8" s="182"/>
+      <c r="AF8" s="182" t="s">
         <v>325</v>
       </c>
-      <c r="AG8" s="208"/>
-      <c r="AH8" s="208"/>
-      <c r="AI8" s="208" t="s">
+      <c r="AG8" s="182"/>
+      <c r="AH8" s="182"/>
+      <c r="AI8" s="182" t="s">
         <v>326</v>
       </c>
-      <c r="AJ8" s="208"/>
-      <c r="AK8" s="208"/>
-      <c r="AL8" s="208"/>
-      <c r="AM8" s="208" t="s">
+      <c r="AJ8" s="182"/>
+      <c r="AK8" s="182"/>
+      <c r="AL8" s="182"/>
+      <c r="AM8" s="182" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:39">
-      <c r="E11" s="205" t="str" cm="1">
+      <c r="E11" s="179" t="str" cm="1">
         <f t="array" ref="E11:E20">_xlfn.TOCOL(E8:AM8,1)</f>
         <v>D</v>
       </c>
-      <c r="F11" s="205" cm="1">
+      <c r="F11" s="179" cm="1">
         <f t="array" aca="1" ref="F11:F20" ca="1">COLUMN(INDIRECT(_xlfn.ANCHORARRAY(E11)&amp;1))</f>
         <v>4</v>
       </c>
-      <c r="G11" s="205">
+      <c r="G11" s="179">
         <f ca="1">F11-1</f>
         <v>3</v>
       </c>
-      <c r="I11" s="205" t="s">
+      <c r="I11" s="179" t="s">
         <v>758</v>
       </c>
-      <c r="J11" s="205" t="s">
+      <c r="J11" s="179" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:39">
-      <c r="E12" s="205" t="str">
+      <c r="E12" s="179" t="str">
         <v>H</v>
       </c>
-      <c r="F12" s="205">
+      <c r="F12" s="179">
         <f ca="1"/>
         <v>8</v>
       </c>
-      <c r="G12" s="205">
+      <c r="G12" s="179">
         <f t="shared" ref="G12:G20" ca="1" si="0">F12-1</f>
         <v>7</v>
       </c>
-      <c r="I12" s="205" t="s">
+      <c r="I12" s="179" t="s">
         <v>759</v>
       </c>
-      <c r="J12" s="205" t="s">
+      <c r="J12" s="179" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="13" spans="1:39">
-      <c r="E13" s="205" t="str">
+      <c r="E13" s="179" t="str">
         <v>M</v>
       </c>
-      <c r="F13" s="205">
+      <c r="F13" s="179">
         <f ca="1"/>
         <v>13</v>
       </c>
-      <c r="G13" s="205">
+      <c r="G13" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
-      <c r="I13" s="205" t="s">
+      <c r="I13" s="179" t="s">
         <v>760</v>
       </c>
-      <c r="J13" s="205" t="s">
+      <c r="J13" s="179" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:39">
-      <c r="E14" s="205" t="str">
+      <c r="E14" s="179" t="str">
         <v>Q</v>
       </c>
-      <c r="F14" s="205">
+      <c r="F14" s="179">
         <f ca="1"/>
         <v>17</v>
       </c>
-      <c r="G14" s="205">
+      <c r="G14" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="I14" s="205" t="s">
+      <c r="I14" s="179" t="s">
         <v>761</v>
       </c>
-      <c r="J14" s="205" t="s">
+      <c r="J14" s="179" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:39">
-      <c r="E15" s="205" t="str">
+      <c r="E15" s="179" t="str">
         <v>T</v>
       </c>
-      <c r="F15" s="205">
+      <c r="F15" s="179">
         <f ca="1"/>
         <v>20</v>
       </c>
-      <c r="G15" s="205">
+      <c r="G15" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="I15" s="205" t="s">
+      <c r="I15" s="179" t="s">
         <v>762</v>
       </c>
-      <c r="J15" s="205" t="s">
+      <c r="J15" s="179" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:39">
-      <c r="E16" s="205" t="str">
+      <c r="E16" s="179" t="str">
         <v>W</v>
       </c>
-      <c r="F16" s="205">
+      <c r="F16" s="179">
         <f ca="1"/>
         <v>23</v>
       </c>
-      <c r="G16" s="205">
+      <c r="G16" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
-      <c r="I16" s="205" t="s">
+      <c r="I16" s="179" t="s">
         <v>763</v>
       </c>
-      <c r="J16" s="205" t="s">
+      <c r="J16" s="179" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="17" spans="5:10">
-      <c r="E17" s="205" t="str">
+      <c r="E17" s="179" t="str">
         <v>AB</v>
       </c>
-      <c r="F17" s="205">
+      <c r="F17" s="179">
         <f ca="1"/>
         <v>28</v>
       </c>
-      <c r="G17" s="205">
+      <c r="G17" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
-      <c r="I17" s="205" t="s">
+      <c r="I17" s="179" t="s">
         <v>764</v>
       </c>
-      <c r="J17" s="205" t="s">
+      <c r="J17" s="179" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" spans="5:10">
-      <c r="E18" s="205" t="str">
+      <c r="E18" s="179" t="str">
         <v>AE</v>
       </c>
-      <c r="F18" s="205">
+      <c r="F18" s="179">
         <f ca="1"/>
         <v>31</v>
       </c>
-      <c r="G18" s="205">
+      <c r="G18" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
-      <c r="I18" s="205" t="s">
+      <c r="I18" s="179" t="s">
         <v>765</v>
       </c>
-      <c r="J18" s="205" t="s">
+      <c r="J18" s="179" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="19" spans="5:10">
-      <c r="E19" s="205" t="str">
+      <c r="E19" s="179" t="str">
         <v>AH</v>
       </c>
-      <c r="F19" s="205">
+      <c r="F19" s="179">
         <f ca="1"/>
         <v>34</v>
       </c>
-      <c r="G19" s="205">
+      <c r="G19" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>33</v>
       </c>
-      <c r="I19" s="205" t="s">
+      <c r="I19" s="179" t="s">
         <v>766</v>
       </c>
-      <c r="J19" s="205" t="s">
+      <c r="J19" s="179" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="5:10">
-      <c r="E20" s="205" t="str">
+      <c r="E20" s="179" t="str">
         <v>AL</v>
       </c>
-      <c r="F20" s="205">
+      <c r="F20" s="179">
         <f ca="1"/>
         <v>38</v>
       </c>
-      <c r="G20" s="205">
+      <c r="G20" s="179">
         <f t="shared" ca="1" si="0"/>
         <v>37</v>
       </c>
-      <c r="I20" s="205" t="s">
+      <c r="I20" s="179" t="s">
         <v>767</v>
       </c>
-      <c r="J20" s="205" t="s">
+      <c r="J20" s="179" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="21" spans="5:10">
-      <c r="G21" s="205">
-        <f ca="1">F11+1</f>
+      <c r="G21" s="179">
+        <f t="shared" ref="G21:G30" ca="1" si="1">F11+1</f>
         <v>5</v>
       </c>
-      <c r="I21" s="205" t="s">
+      <c r="I21" s="179" t="s">
         <v>753</v>
       </c>
-      <c r="J21" s="205" t="s">
+      <c r="J21" s="179" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="22" spans="5:10">
-      <c r="G22" s="205">
-        <f ca="1">F12+1</f>
+      <c r="G22" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="I22" s="205" t="s">
+      <c r="I22" s="179" t="s">
         <v>756</v>
       </c>
-      <c r="J22" s="205" t="s">
+      <c r="J22" s="179" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="23" spans="5:10">
-      <c r="G23" s="205">
-        <f ca="1">F13+1</f>
+      <c r="G23" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
-      <c r="I23" s="205" t="s">
+      <c r="I23" s="179" t="s">
         <v>757</v>
       </c>
-      <c r="J23" s="205" t="s">
+      <c r="J23" s="179" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="24" spans="5:10">
-      <c r="G24" s="205">
-        <f ca="1">F14+1</f>
+      <c r="G24" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
-      <c r="I24" s="205" t="s">
+      <c r="I24" s="179" t="s">
         <v>768</v>
       </c>
-      <c r="J24" s="205" t="s">
+      <c r="J24" s="179" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="25" spans="5:10">
-      <c r="G25" s="205">
-        <f ca="1">F15+1</f>
+      <c r="G25" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="205" t="s">
+      <c r="I25" s="179" t="s">
         <v>769</v>
       </c>
-      <c r="J25" s="205" t="s">
+      <c r="J25" s="179" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="5:10">
-      <c r="G26" s="205">
-        <f ca="1">F16+1</f>
+      <c r="G26" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
-      <c r="I26" s="205" t="s">
+      <c r="I26" s="179" t="s">
         <v>770</v>
       </c>
-      <c r="J26" s="205" t="s">
+      <c r="J26" s="179" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="27" spans="5:10">
-      <c r="G27" s="205">
-        <f ca="1">F17+1</f>
+      <c r="G27" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
-      <c r="I27" s="205" t="s">
+      <c r="I27" s="179" t="s">
         <v>771</v>
       </c>
-      <c r="J27" s="205" t="s">
+      <c r="J27" s="179" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="28" spans="5:10">
-      <c r="G28" s="205">
-        <f ca="1">F18+1</f>
+      <c r="G28" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>32</v>
       </c>
-      <c r="I28" s="205" t="s">
+      <c r="I28" s="179" t="s">
         <v>772</v>
       </c>
-      <c r="J28" s="205" t="s">
+      <c r="J28" s="179" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="29" spans="5:10">
-      <c r="G29" s="205">
-        <f ca="1">F19+1</f>
+      <c r="G29" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>35</v>
       </c>
-      <c r="I29" s="205" t="s">
+      <c r="I29" s="179" t="s">
         <v>773</v>
       </c>
-      <c r="J29" s="205" t="s">
+      <c r="J29" s="179" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="30" spans="5:10">
-      <c r="G30" s="205">
-        <f ca="1">F20+1</f>
+      <c r="G30" s="179">
+        <f t="shared" ca="1" si="1"/>
         <v>39</v>
       </c>
-      <c r="I30" s="205" t="s">
+      <c r="I30" s="179" t="s">
         <v>774</v>
       </c>
-      <c r="J30" s="205" t="s">
+      <c r="J30" s="179" t="s">
         <v>143</v>
       </c>
     </row>
@@ -19556,10 +19556,10 @@
       <c r="AM1" s="79"/>
       <c r="AN1" s="79"/>
       <c r="AO1" s="80"/>
-      <c r="AQ1" s="203" t="s">
+      <c r="AQ1" s="201" t="s">
         <v>328</v>
       </c>
-      <c r="AR1" s="204"/>
+      <c r="AR1" s="202"/>
     </row>
     <row r="2" spans="1:45" ht="16.95" customHeight="1" thickBot="1">
       <c r="A2" s="82"/>
@@ -23397,10 +23397,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.8" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="187" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="185"/>
+      <c r="B1" s="189"/>
       <c r="C1" s="153"/>
     </row>
     <row r="2" spans="1:3" ht="16.8" customHeight="1">
@@ -23593,10 +23593,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="187" t="s">
         <v>357</v>
       </c>
-      <c r="B1" s="185"/>
+      <c r="B1" s="189"/>
       <c r="C1" s="153"/>
       <c r="D1" s="153"/>
     </row>
@@ -24009,11 +24009,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="187" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="185"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="189"/>
       <c r="D1" s="71"/>
     </row>
     <row r="2" spans="1:4" ht="36.6" customHeight="1">
@@ -28164,8 +28164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB505C8-B5A5-43E7-BDB1-CEB8314A9C64}">
   <dimension ref="A1:AA327"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I125" sqref="I125"/>
+    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -28184,39 +28184,39 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" customHeight="1"/>
     <row r="2" spans="2:16" ht="59.25" customHeight="1">
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="190" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193"/>
-      <c r="L2" s="193"/>
-      <c r="M2" s="194"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="192"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1"/>
     <row r="4" spans="2:16" ht="33" customHeight="1">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="187" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="185"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="189"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="183" t="s">
+      <c r="L4" s="187" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="185"/>
+      <c r="M4" s="189"/>
     </row>
     <row r="5" spans="2:16" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -28229,10 +28229,10 @@
       <c r="P5"/>
     </row>
     <row r="6" spans="2:16" ht="33" customHeight="1">
-      <c r="L6" s="183" t="s">
+      <c r="L6" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="185"/>
+      <c r="M6" s="189"/>
     </row>
     <row r="7" spans="2:16" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -28240,52 +28240,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="196"/>
-      <c r="K8" s="196"/>
-      <c r="L8" s="196"/>
-      <c r="M8" s="196"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="194"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="194"/>
+      <c r="L8" s="194"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="2:16" ht="162" customHeight="1">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="195" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="197"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="197"/>
-      <c r="M9" s="197"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
+      <c r="I9" s="195"/>
+      <c r="J9" s="195"/>
+      <c r="K9" s="195"/>
+      <c r="L9" s="195"/>
+      <c r="M9" s="195"/>
     </row>
     <row r="10" spans="2:16" ht="245.4" customHeight="1">
-      <c r="B10" s="198" t="s">
+      <c r="B10" s="196" t="s">
         <v>727</v>
       </c>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
-      <c r="F10" s="198"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="198"/>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
-      <c r="K10" s="198"/>
-      <c r="L10" s="198"/>
-      <c r="M10" s="198"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="196"/>
+      <c r="J10" s="196"/>
+      <c r="K10" s="196"/>
+      <c r="L10" s="196"/>
+      <c r="M10" s="196"/>
     </row>
     <row r="11" spans="2:16" ht="15" customHeight="1">
       <c r="B11" s="5"/>
@@ -28302,20 +28302,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:16" ht="21.75" customHeight="1">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="187" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="185"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="188"/>
+      <c r="H12" s="188"/>
+      <c r="I12" s="188"/>
+      <c r="J12" s="188"/>
+      <c r="K12" s="188"/>
+      <c r="L12" s="188"/>
+      <c r="M12" s="189"/>
     </row>
     <row r="13" spans="2:16" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -28365,15 +28365,15 @@
         <v>86</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="199" t="s">
+      <c r="G16" s="197" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="200"/>
-      <c r="I16" s="200"/>
-      <c r="J16" s="200"/>
-      <c r="K16" s="200"/>
-      <c r="L16" s="200"/>
-      <c r="M16" s="201"/>
+      <c r="H16" s="198"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="198"/>
+      <c r="K16" s="198"/>
+      <c r="L16" s="198"/>
+      <c r="M16" s="199"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="16" t="s">
@@ -28392,15 +28392,15 @@
         <f>IF(ISBLANK(Case!E17),0,IF(E17=Case!E17,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="202" t="s">
+      <c r="G17" s="200" t="s">
         <v>732</v>
       </c>
-      <c r="H17" s="202"/>
-      <c r="I17" s="202"/>
-      <c r="J17" s="202"/>
-      <c r="K17" s="202"/>
-      <c r="L17" s="202"/>
-      <c r="M17" s="202"/>
+      <c r="H17" s="200"/>
+      <c r="I17" s="200"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="200"/>
+      <c r="M17" s="200"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="16" t="s">
@@ -28419,15 +28419,15 @@
         <f>IF(ISBLANK(Case!E18),0,IF(E18=Case!E18,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="179" t="s">
+      <c r="G18" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="179"/>
-      <c r="J18" s="179"/>
-      <c r="K18" s="179"/>
-      <c r="L18" s="179"/>
-      <c r="M18" s="179"/>
+      <c r="H18" s="183"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="183"/>
+      <c r="K18" s="183"/>
+      <c r="L18" s="183"/>
+      <c r="M18" s="183"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="16" t="s">
@@ -28446,15 +28446,15 @@
         <f>IF(ISBLANK(Case!E19),0,IF(E19=Case!E19,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="179" t="s">
+      <c r="G19" s="183" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="179"/>
-      <c r="I19" s="179"/>
-      <c r="J19" s="179"/>
-      <c r="K19" s="179"/>
-      <c r="L19" s="179"/>
-      <c r="M19" s="179"/>
+      <c r="H19" s="183"/>
+      <c r="I19" s="183"/>
+      <c r="J19" s="183"/>
+      <c r="K19" s="183"/>
+      <c r="L19" s="183"/>
+      <c r="M19" s="183"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="16" t="s">
@@ -28473,15 +28473,15 @@
         <f>IF(ISBLANK(Case!E20),0,IF(E20=Case!E20,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="179" t="s">
+      <c r="G20" s="183" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="179"/>
-      <c r="I20" s="179"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="179"/>
-      <c r="L20" s="179"/>
-      <c r="M20" s="179"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+      <c r="K20" s="183"/>
+      <c r="L20" s="183"/>
+      <c r="M20" s="183"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="16" t="s">
@@ -28500,34 +28500,34 @@
         <f>IF(ISBLANK(Case!E21),0,IF(E21=Case!E21,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="180" t="s">
+      <c r="G21" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="J21" s="181"/>
-      <c r="K21" s="181"/>
-      <c r="L21" s="181"/>
-      <c r="M21" s="182"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
+      <c r="M21" s="186"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="187" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="184"/>
-      <c r="D23" s="184"/>
-      <c r="E23" s="184"/>
-      <c r="F23" s="184"/>
-      <c r="G23" s="184"/>
-      <c r="H23" s="184"/>
-      <c r="I23" s="184"/>
-      <c r="J23" s="184"/>
-      <c r="K23" s="184"/>
-      <c r="L23" s="184"/>
-      <c r="M23" s="185"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
+      <c r="K23" s="188"/>
+      <c r="L23" s="188"/>
+      <c r="M23" s="189"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -28553,21 +28553,21 @@
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
       <c r="F25" s="20"/>
-      <c r="L25" s="183" t="s">
+      <c r="L25" s="187" t="s">
         <v>735</v>
       </c>
-      <c r="M25" s="185"/>
+      <c r="M25" s="189"/>
     </row>
     <row r="26" spans="2:13" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B26" s="29"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
-      <c r="L26" s="186">
+      <c r="L26" s="203">
         <f>SUMPRODUCT(--(F:F=1),D:D)</f>
         <v>620</v>
       </c>
-      <c r="M26" s="187"/>
+      <c r="M26" s="204"/>
     </row>
     <row r="27" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B27" s="28" t="s">
@@ -28577,8 +28577,8 @@
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="L27" s="188"/>
-      <c r="M27" s="189"/>
+      <c r="L27" s="205"/>
+      <c r="M27" s="206"/>
     </row>
     <row r="28" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B28" s="29"/>
@@ -28586,8 +28586,8 @@
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="L28" s="190"/>
-      <c r="M28" s="191"/>
+      <c r="L28" s="207"/>
+      <c r="M28" s="208"/>
     </row>
     <row r="29" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B29" s="31" t="s">
@@ -31279,20 +31279,20 @@
       <c r="K147" s="67"/>
     </row>
     <row r="148" spans="1:27" ht="23.4">
-      <c r="B148" s="183" t="s">
+      <c r="B148" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="C148" s="184"/>
-      <c r="D148" s="184"/>
-      <c r="E148" s="184"/>
-      <c r="F148" s="184"/>
-      <c r="G148" s="184"/>
-      <c r="H148" s="184"/>
-      <c r="I148" s="184"/>
-      <c r="J148" s="184"/>
-      <c r="K148" s="184"/>
-      <c r="L148" s="184"/>
-      <c r="M148" s="185"/>
+      <c r="C148" s="188"/>
+      <c r="D148" s="188"/>
+      <c r="E148" s="188"/>
+      <c r="F148" s="188"/>
+      <c r="G148" s="188"/>
+      <c r="H148" s="188"/>
+      <c r="I148" s="188"/>
+      <c r="J148" s="188"/>
+      <c r="K148" s="188"/>
+      <c r="L148" s="188"/>
+      <c r="M148" s="189"/>
     </row>
     <row r="149" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="B149" s="24"/>
@@ -33246,20 +33246,20 @@
       <c r="K232" s="67"/>
     </row>
     <row r="233" spans="1:27" ht="23.4">
-      <c r="B233" s="183" t="s">
+      <c r="B233" s="187" t="s">
         <v>211</v>
       </c>
-      <c r="C233" s="184"/>
-      <c r="D233" s="184"/>
-      <c r="E233" s="184"/>
-      <c r="F233" s="184"/>
-      <c r="G233" s="184"/>
-      <c r="H233" s="184"/>
-      <c r="I233" s="184"/>
-      <c r="J233" s="184"/>
-      <c r="K233" s="184"/>
-      <c r="L233" s="184"/>
-      <c r="M233" s="185"/>
+      <c r="C233" s="188"/>
+      <c r="D233" s="188"/>
+      <c r="E233" s="188"/>
+      <c r="F233" s="188"/>
+      <c r="G233" s="188"/>
+      <c r="H233" s="188"/>
+      <c r="I233" s="188"/>
+      <c r="J233" s="188"/>
+      <c r="K233" s="188"/>
+      <c r="L233" s="188"/>
+      <c r="M233" s="189"/>
     </row>
     <row r="234" spans="1:27" ht="15" customHeight="1" thickBot="1">
       <c r="B234" s="24"/>
@@ -35367,6 +35367,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B148:M148"/>
+    <mergeCell ref="B233:M233"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M28"/>
     <mergeCell ref="G19:M19"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B4:J4"/>
@@ -35379,13 +35386,6 @@
     <mergeCell ref="G16:M16"/>
     <mergeCell ref="G17:M17"/>
     <mergeCell ref="G18:M18"/>
-    <mergeCell ref="G20:M20"/>
-    <mergeCell ref="G21:M21"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B148:M148"/>
-    <mergeCell ref="B233:M233"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>